<commit_message>
Lees gegevens direct uit excel
</commit_message>
<xml_diff>
--- a/roulette2025.xlsx
+++ b/roulette2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tacobakker/PycharmProjects/Kitchenroulette/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0515D5FC-E6BB-404E-8B86-CDE922813610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F815FA0-E97F-C44C-A276-BB919FB31DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="2960" windowWidth="27440" windowHeight="16240" xr2:uid="{00D46D12-6840-BD4A-9AFF-D7800ADFA46E}"/>
+    <workbookView xWindow="7360" yWindow="3720" windowWidth="27440" windowHeight="16240" xr2:uid="{00D46D12-6840-BD4A-9AFF-D7800ADFA46E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -48,15 +48,9 @@
     <t>voorgerecht</t>
   </si>
   <si>
-    <t>hoofgerecht</t>
-  </si>
-  <si>
     <t>nagerecht</t>
   </si>
   <si>
-    <t>aantal personen</t>
-  </si>
-  <si>
     <t>dieetwensen</t>
   </si>
   <si>
@@ -192,7 +186,13 @@
     <t>Geen paprika</t>
   </si>
   <si>
-    <t>max aantal eters</t>
+    <t>hoofdgerecht</t>
+  </si>
+  <si>
+    <t>aantalpersonen</t>
+  </si>
+  <si>
+    <t>maxaantaleters</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -599,7 +599,8 @@
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="61.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -612,438 +613,438 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3">
         <v>8</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3">
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3">
-        <v>8</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G12" s="3">
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G13" s="3">
         <v>8</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="3">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="G14" s="3">
-        <v>8</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" s="3">
         <v>6</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" s="3">
         <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G17" s="3">
         <v>6</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1063,418 +1064,418 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
         <v>9</v>
-      </c>
-      <c r="G13">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>